<commit_message>
Added user_agent details for each browser
</commit_message>
<xml_diff>
--- a/web-scraping/settings/headers.xlsx
+++ b/web-scraping/settings/headers.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/neil/Documents/training/data-analytics/data-analytics-portfolio/web-scraping/settings/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56A0CE82-28AD-2D40-9077-68D19FE95422}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDE53873-2D3B-8449-ACFF-84C62BF5948F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="33820" windowHeight="18080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="31540" yWindow="8860" windowWidth="33820" windowHeight="18080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1 - headers" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="20">
   <si>
     <t>os</t>
   </si>
@@ -50,13 +50,43 @@
   </si>
   <si>
     <t>windows</t>
+  </si>
+  <si>
+    <t>Mozilla/5.0 (Macintosh; Intel Mac OS X 10_15_7) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/116.0.0.0 Safari/537.36</t>
+  </si>
+  <si>
+    <t>Mozilla/5.0 (Windows NT 10.0; Win64; x64) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/116.0.0.0 Safari/537.36</t>
+  </si>
+  <si>
+    <t>Mozilla/5.0 (X11; Linux x86_64) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/116.0.0.0 Safari/537.36</t>
+  </si>
+  <si>
+    <t>Mozilla/5.0 (Windows NT 10.0; Win64; x64; rv:109.0) Gecko/20100101 Firefox/117.0</t>
+  </si>
+  <si>
+    <t>Mozilla/5.0 (Macintosh; Intel Mac OS X 10_15_7) AppleWebKit/605.1.15 (KHTML, like Gecko) Version/16.6 Safari/605.1.15</t>
+  </si>
+  <si>
+    <t>Mozilla/5.0 (X11; Linux x86_64; rv:109.0) Gecko/20100101 Firefox/117.0</t>
+  </si>
+  <si>
+    <t>Mozilla/5.0 (Macintosh; Intel Mac OS X 10.15; rv:109.0) Gecko/20100101 Firefox/117.0</t>
+  </si>
+  <si>
+    <t>Mozilla/5.0 (Windows NT 10.0; Win64; x64) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/114.0.0.0 Safari/537.36 Edg/114.0.1823.106</t>
+  </si>
+  <si>
+    <t>Mozilla/5.0 (X11; Linux x86_64) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/114.0.0.0 Safari/537.36 Edg/114.0.1823.106</t>
+  </si>
+  <si>
+    <t>Mozilla/5.0 (Macintosh; Intel Mac OS X 10_15_7) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/114.0.0.0 Safari/537.36 Edg/114.0.1823.106</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
@@ -64,6 +94,12 @@
     </font>
     <font>
       <b/>
+      <sz val="10"/>
+      <color indexed="8"/>
+      <name val="Helvetica Neue"/>
+      <family val="2"/>
+    </font>
+    <font>
       <sz val="10"/>
       <color indexed="8"/>
       <name val="Helvetica Neue"/>
@@ -92,7 +128,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -106,6 +142,9 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
   </cellXfs>
@@ -1240,9 +1279,7 @@
   </sheetPr>
   <dimension ref="A1:D12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="220" zoomScaleNormal="220" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.33203125" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
@@ -1272,8 +1309,8 @@
       <c r="B2" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="3">
-        <v>1</v>
+      <c r="C2" s="5" t="s">
+        <v>12</v>
       </c>
       <c r="D2" s="3"/>
     </row>
@@ -1284,8 +1321,8 @@
       <c r="B3" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="3">
-        <v>2</v>
+      <c r="C3" s="5" t="s">
+        <v>18</v>
       </c>
       <c r="D3" s="3"/>
     </row>
@@ -1296,8 +1333,8 @@
       <c r="B4" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="3">
-        <v>3</v>
+      <c r="C4" s="5" t="s">
+        <v>15</v>
       </c>
       <c r="D4" s="3"/>
     </row>
@@ -1308,8 +1345,8 @@
       <c r="B5" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="3">
-        <v>4</v>
+      <c r="C5" s="5" t="s">
+        <v>10</v>
       </c>
       <c r="D5" s="3"/>
     </row>
@@ -1320,8 +1357,8 @@
       <c r="B6" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="3">
-        <v>5</v>
+      <c r="C6" s="5" t="s">
+        <v>19</v>
       </c>
       <c r="D6" s="3"/>
     </row>
@@ -1332,8 +1369,8 @@
       <c r="B7" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="3">
-        <v>6</v>
+      <c r="C7" s="5" t="s">
+        <v>16</v>
       </c>
       <c r="D7" s="3"/>
     </row>
@@ -1344,8 +1381,8 @@
       <c r="B8" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="3">
-        <v>7</v>
+      <c r="C8" s="5" t="s">
+        <v>14</v>
       </c>
       <c r="D8" s="3"/>
     </row>
@@ -1356,8 +1393,8 @@
       <c r="B9" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C9" s="3">
-        <v>8</v>
+      <c r="C9" s="5" t="s">
+        <v>11</v>
       </c>
       <c r="D9" s="3"/>
     </row>
@@ -1368,8 +1405,8 @@
       <c r="B10" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C10" s="3">
-        <v>9</v>
+      <c r="C10" s="5" t="s">
+        <v>17</v>
       </c>
       <c r="D10" s="3"/>
     </row>
@@ -1380,8 +1417,8 @@
       <c r="B11" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C11" s="3">
-        <v>0</v>
+      <c r="C11" s="5" t="s">
+        <v>13</v>
       </c>
       <c r="D11" s="3"/>
     </row>

</xml_diff>